<commit_message>
a few changes to get the code working
+plus second iteration, I don't remember what limit features in vector matrix is though
</commit_message>
<xml_diff>
--- a/Results assignment 2.xlsx
+++ b/Results assignment 2.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvits\OneDrive\Desktop\2024\Uni\NLP\package install\Assignment2Repo\Natural_Language_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BE3779-CF08-4062-B041-5E0E9CFDF998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449D30AE-62B8-4180-A30A-D721E732FBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="1356" windowWidth="13956" windowHeight="10524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13500" yWindow="2055" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -378,15 +389,15 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -397,12 +408,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -416,7 +427,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -430,7 +441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -444,12 +455,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -460,10 +471,10 @@
         <v>0.46</v>
       </c>
       <c r="D8">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -474,10 +485,10 @@
         <v>0.98</v>
       </c>
       <c r="D9">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -488,45 +499,46 @@
         <v>0.45600000000000002</v>
       </c>
       <c r="D10">
-        <v>0.622</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <f>D8*D9</f>
+        <v>0.65280000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>

</xml_diff>